<commit_message>
Updated current progress of benchmarking runs
</commit_message>
<xml_diff>
--- a/benchmarking_progress.xlsx
+++ b/benchmarking_progress.xlsx
@@ -8,25 +8,89 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552154C6-2F35-4B2D-B757-6ED4C065A907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A82C18-6CBF-4B1B-BE9F-DDD0CDAA27F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="450" windowWidth="21945" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="1440" windowWidth="15000" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SBS_down_samp" sheetId="1" r:id="rId1"/>
     <sheet name="indel_down_samp" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A1CE78B5-9DF1-4968-B7D0-A71C55FBB491}</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{A1CE78B5-9DF1-4968-B7D0-A71C55FBB491}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Running on monster2</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6E6D9F0A-B5DA-4B73-B14C-831655C72B6E}</author>
+    <author>tc={6952DBC2-D2FB-4011-BDCF-30BF10CB5F2A}</author>
+    <author>tc={449C874C-BE33-429C-9820-309BE9010AC0}</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{6E6D9F0A-B5DA-4B73-B14C-831655C72B6E}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Ignore 500, 1k, 10k right now</t>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="1" shapeId="0" xr:uid="{6952DBC2-D2FB-4011-BDCF-30BF10CB5F2A}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Running on new HPC cluster</t>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="2" shapeId="0" xr:uid="{449C874C-BE33-429C-9820-309BE9010AC0}">
+      <text>
+        <t>[线程批注]
+你的Excel版本可读取此线程批注; 但如果在更新版本的Excel中打开文件，则对批注所作的任何改动都将被删除。了解详细信息: https://go.microsoft.com/fwlink/?linkid=870924
+注释:
+    Running on monster2</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -94,14 +158,17 @@
     <t>10.1101/2022.01.31.478587v1</t>
   </si>
   <si>
-    <t>** Green - running; Red - failed; White - not running;</t>
+    <t>hdp-NR-</t>
+  </si>
+  <si>
+    <t>** Filling colors: Green - running; Red - failed; White - not running;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +192,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -162,9 +250,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -177,13 +262,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -201,6 +298,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Wu Yang" id="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" userId="Wu Yang" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,15 +567,37 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F3" dT="2022-06-23T10:45:35.89" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{A1CE78B5-9DF1-4968-B7D0-A71C55FBB491}">
+    <text>Running on monster2</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H2" dT="2022-06-23T07:17:23.70" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{6E6D9F0A-B5DA-4B73-B14C-831655C72B6E}">
+    <text>Ignore 500, 1k, 10k right now</text>
+  </threadedComment>
+  <threadedComment ref="D3" dT="2022-06-25T23:15:02.23" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{6952DBC2-D2FB-4011-BDCF-30BF10CB5F2A}">
+    <text>Running on new HPC cluster</text>
+  </threadedComment>
+  <threadedComment ref="D4" dT="2022-06-23T10:45:19.33" personId="{AB773AB3-621A-4D8C-80C6-159025BBDEEC}" id="{449C874C-BE33-429C-9820-309BE9010AC0}">
+    <text>Running on monster2</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,19 +614,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -513,22 +638,22 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -540,7 +665,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2022</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -549,25 +674,25 @@
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8">
         <v>3</v>
       </c>
-      <c r="E3" s="10">
+      <c r="G3" s="8">
         <v>3</v>
       </c>
-      <c r="F3" s="10">
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -575,7 +700,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2022</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -584,86 +709,88 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="D4" s="9">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -675,18 +802,19 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCBB4E0-5F89-431B-A9E8-4B03CB92E69C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCBB4E0-5F89-431B-A9E8-4B03CB92E69C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,19 +831,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -733,16 +861,16 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -754,7 +882,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>2022</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -763,15 +891,25 @@
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4" t="s">
+      <c r="D3" s="9">
+        <v>5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9">
+        <v>5</v>
+      </c>
+      <c r="G3" s="9">
+        <v>5</v>
+      </c>
+      <c r="H3" s="9">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -779,7 +917,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2022</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -788,86 +926,86 @@
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="D4" s="9">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9">
+        <v>5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -879,5 +1017,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>